<commit_message>
final code backend and frontend
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_1_uk_january2026.xlsx
+++ b/backend/uploads/currentinventory_1_uk_january2026.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Sno.</t>
   </si>
@@ -124,6 +124,12 @@
     <t>SEIWHCMEWI</t>
   </si>
   <si>
+    <t>25-954C-QWS0</t>
+  </si>
+  <si>
+    <t>SEIWBW</t>
+  </si>
+  <si>
     <t>Classic</t>
   </si>
   <si>
@@ -164,6 +170,12 @@
   </si>
   <si>
     <t>Wipes + Menthol</t>
+  </si>
+  <si>
+    <t>New Wipes</t>
+  </si>
+  <si>
+    <t>Body Wash</t>
   </si>
   <si>
     <t>Total</t>
@@ -524,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -606,16 +618,16 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4588</v>
+        <v>4531</v>
       </c>
       <c r="K2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L2">
         <v>6</v>
@@ -624,31 +636,31 @@
         <v>10</v>
       </c>
       <c r="N2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O2">
-        <v>4613</v>
+        <v>4537</v>
       </c>
       <c r="P2">
-        <v>4122</v>
+        <v>4286</v>
       </c>
       <c r="Q2">
-        <v>511.68</v>
+        <v>504.85</v>
       </c>
       <c r="R2">
-        <v>4588</v>
+        <v>3974</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>558</v>
       </c>
       <c r="V2">
-        <v>4588</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -659,37 +671,37 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="K3">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="L3">
-        <v>242</v>
+        <v>290</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O3">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="P3">
-        <v>38350</v>
+        <v>33101</v>
       </c>
       <c r="Q3">
-        <v>71.45</v>
+        <v>70.73</v>
       </c>
       <c r="R3">
-        <v>844</v>
+        <v>772</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -698,10 +710,10 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="V3">
-        <v>844</v>
+        <v>838</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -712,13 +724,13 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -736,13 +748,13 @@
         <v>232</v>
       </c>
       <c r="P4">
-        <v>35611</v>
+        <v>46507</v>
       </c>
       <c r="Q4">
-        <v>31.45</v>
+        <v>30.69</v>
       </c>
       <c r="R4">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -751,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="V4">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -765,13 +777,13 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -786,16 +798,16 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P5">
-        <v>143228</v>
+        <v>148209</v>
       </c>
       <c r="Q5">
-        <v>8.029999999999999</v>
+        <v>7.88</v>
       </c>
       <c r="R5">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -804,10 +816,10 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V5">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -818,19 +830,19 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -842,13 +854,13 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>27236</v>
+        <v>23989</v>
       </c>
       <c r="Q6">
-        <v>32.43</v>
+        <v>31.77</v>
       </c>
       <c r="R6">
-        <v>263</v>
+        <v>216</v>
       </c>
       <c r="S6">
         <v>0</v>
@@ -857,10 +869,10 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="V6">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -871,19 +883,19 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="K7">
         <v>43</v>
       </c>
       <c r="L7">
-        <v>769</v>
+        <v>749</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -895,13 +907,13 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>10367</v>
+        <v>10746</v>
       </c>
       <c r="Q7">
-        <v>92.95</v>
+        <v>91.12</v>
       </c>
       <c r="R7">
-        <v>793</v>
+        <v>631</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -910,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="V7">
-        <v>793</v>
+        <v>779</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -924,7 +936,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -948,13 +960,13 @@
         <v>313</v>
       </c>
       <c r="P8">
-        <v>151489</v>
+        <v>157552</v>
       </c>
       <c r="Q8">
-        <v>35.75</v>
+        <v>35.74</v>
       </c>
       <c r="R8">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -963,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="V8">
         <v>318</v>
@@ -977,7 +989,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1009,22 +1021,22 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="K10">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="L10">
-        <v>774</v>
+        <v>828</v>
       </c>
       <c r="M10">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1033,13 +1045,13 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>4122</v>
+        <v>4286</v>
       </c>
       <c r="Q10">
-        <v>113.04</v>
+        <v>112.43</v>
       </c>
       <c r="R10">
-        <v>949</v>
+        <v>866</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -1048,10 +1060,10 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="V10">
-        <v>949</v>
+        <v>944</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1062,19 +1074,19 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1056</v>
+        <v>1051</v>
       </c>
       <c r="K11">
         <v>92</v>
       </c>
       <c r="L11">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1086,13 +1098,13 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>4122</v>
+        <v>4286</v>
       </c>
       <c r="Q11">
-        <v>98.22</v>
+        <v>97.64</v>
       </c>
       <c r="R11">
-        <v>1056</v>
+        <v>929</v>
       </c>
       <c r="S11">
         <v>0</v>
@@ -1101,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="V11">
-        <v>1056</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1115,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1142,10 +1154,10 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>61.92</v>
+        <v>61.91</v>
       </c>
       <c r="R12">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -1154,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V12">
         <v>507</v>
@@ -1168,13 +1180,13 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K13">
         <v>6</v>
@@ -1192,13 +1204,13 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>124829</v>
+        <v>165150</v>
       </c>
       <c r="Q13">
-        <v>20.1</v>
+        <v>19.88</v>
       </c>
       <c r="R13">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -1207,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V13">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1221,7 +1233,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1253,7 +1265,7 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1262,10 +1274,10 @@
         <v>141</v>
       </c>
       <c r="K15">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L15">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1277,13 +1289,13 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>97001</v>
+        <v>112992</v>
       </c>
       <c r="Q15">
-        <v>42.55</v>
+        <v>42.53</v>
       </c>
       <c r="R15">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -1292,45 +1304,51 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="V15">
         <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:22">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>9854</v>
+        <v>885</v>
       </c>
       <c r="K16">
-        <v>486</v>
+        <v>154</v>
       </c>
       <c r="L16">
-        <v>3637</v>
+        <v>630</v>
       </c>
       <c r="M16">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="N16">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>5671</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>640477</v>
+        <v>23989</v>
       </c>
       <c r="Q16">
-        <v>1119.57</v>
+        <v>76.12</v>
       </c>
       <c r="R16">
-        <v>9854</v>
+        <v>784</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1339,10 +1357,110 @@
         <v>0</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="V16">
-        <v>9854</v>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>83</v>
+      </c>
+      <c r="K17">
+        <v>83</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>54783</v>
+      </c>
+      <c r="Q17">
+        <v>6.16</v>
+      </c>
+      <c r="R17">
+        <v>47</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>36</v>
+      </c>
+      <c r="V17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>10723</v>
+      </c>
+      <c r="K18">
+        <v>616</v>
+      </c>
+      <c r="L18">
+        <v>4350</v>
+      </c>
+      <c r="M18">
+        <v>247</v>
+      </c>
+      <c r="N18">
+        <v>25</v>
+      </c>
+      <c r="O18">
+        <v>5590</v>
+      </c>
+      <c r="P18">
+        <v>789876</v>
+      </c>
+      <c r="Q18">
+        <v>1189.45</v>
+      </c>
+      <c r="R18">
+        <v>9487</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>1237</v>
+      </c>
+      <c r="V18">
+        <v>10723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>